<commit_message>
reporte 15 - 21 Junio!
</commit_message>
<xml_diff>
--- a/public/reports/Reporte_Avenue_Polanco.xlsx
+++ b/public/reports/Reporte_Avenue_Polanco.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergirams/Development/Kiper/backend/apikiper/public/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA8AB9B8-344A-F54D-A9B5-44244ED58FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAE98543-C464-D348-87A6-2463DFB89226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="117">
   <si>
     <t>Reporte Oficina de Ventas</t>
   </si>
   <si>
-    <t>8-14 de Junio del 2020</t>
+    <t>15 - 21 de Junio del 2020</t>
   </si>
   <si>
     <t>Reporte Ejecutivo</t>
@@ -88,341 +96,233 @@
     <t>Alejandra Campos García</t>
   </si>
   <si>
-    <t>2020-06-13 22:18:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana molina </t>
-  </si>
-  <si>
-    <t>anashml@gmail.com</t>
+    <t>2020-06-20 15:41:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leticia Rodríguez Peña </t>
+  </si>
+  <si>
+    <t>rho.alrp@gmail.com</t>
+  </si>
+  <si>
+    <t>Envié correo para conocer que necesita.</t>
+  </si>
+  <si>
+    <t>2020-06-20 11:23:40</t>
+  </si>
+  <si>
+    <t>Meredith Monserrat Pineda Serrano</t>
+  </si>
+  <si>
+    <t>mere_pene_serrano@outlook.com</t>
   </si>
   <si>
     <t>Belora Abadi Husny</t>
   </si>
   <si>
-    <t>2020-06-13 19:54:28</t>
-  </si>
-  <si>
-    <t>Diana Enriquez Cisneros</t>
-  </si>
-  <si>
-    <t>de37353@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-13 15:59:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anel Diez Rodriguez </t>
-  </si>
-  <si>
-    <t>contacto@aneldiez.com</t>
-  </si>
-  <si>
-    <t>2020-06-13 15:53:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jhovanny Contreras Hernandez </t>
-  </si>
-  <si>
-    <t>jhova567@icloud.com</t>
-  </si>
-  <si>
-    <t>2020-06-13 13:34:36</t>
-  </si>
-  <si>
-    <t>Cynthia Echeverria</t>
-  </si>
-  <si>
-    <t>5548801304@phnoecall.com</t>
-  </si>
-  <si>
-    <t>Es Broker externa, estoy en espera de que diga que busca su cliente para enviar cotizaciones</t>
-  </si>
-  <si>
-    <t>2020-06-13 12:17:53</t>
-  </si>
-  <si>
-    <t>santi21pa@hotmail.es</t>
-  </si>
-  <si>
-    <t>2020-06-13 09:43:01</t>
-  </si>
-  <si>
-    <t>Zurisadai Ramírez Ballesteros</t>
-  </si>
-  <si>
-    <t>zuriramirez169@gmail.com</t>
-  </si>
-  <si>
-    <t>Envié correo para saber que busca</t>
-  </si>
-  <si>
-    <t>2020-06-13 08:28:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luis Sosa </t>
-  </si>
-  <si>
-    <t>luis.sosa.cb03@gmail.com</t>
-  </si>
-  <si>
-    <t>Envié correo para conocer que busca</t>
-  </si>
-  <si>
-    <t>2020-06-12 21:47:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flavio </t>
-  </si>
-  <si>
-    <t>barchettivalerf@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-12 20:53:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diego Alexis Grajales Becerril </t>
-  </si>
-  <si>
-    <t>dg311204@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-12 20:14:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allan Nuñez </t>
-  </si>
-  <si>
-    <t>allan01paul@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-12 19:14:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Italia Sanchez Naranjo </t>
-  </si>
-  <si>
-    <t>italynaranjo574@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-12 11:07:19</t>
-  </si>
-  <si>
-    <t>m_ortega@toyotacancun.com.mx</t>
-  </si>
-  <si>
-    <t>2020-06-12 08:21:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marcela Karren </t>
-  </si>
-  <si>
-    <t>marcelakarrenv@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-12 07:30:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saul Figueroa </t>
-  </si>
-  <si>
-    <t>Nopidan@datos.com</t>
+    <t>2020-06-20 11:16:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varas Guillermo </t>
+  </si>
+  <si>
+    <t>fguillermovaras@hotmail.com</t>
   </si>
   <si>
     <t>Se envió correo desde Kiper.</t>
   </si>
   <si>
-    <t>2020-06-12 03:36:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria Teresa Verduzco Vázquez </t>
-  </si>
-  <si>
-    <t>tverduzco@hotmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-11 12:25:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diego cervantes de avila </t>
-  </si>
-  <si>
-    <t>Diego_c@hotmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-11 10:53:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Rodríguez </t>
-  </si>
-  <si>
-    <t>coli_gg@hotmail.com</t>
-  </si>
-  <si>
-    <t>Envié correo para preguntar que necesita</t>
-  </si>
-  <si>
-    <t>2020-06-11 08:39:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marcela </t>
-  </si>
-  <si>
-    <t>anasooro@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-11 02:17:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge Alberto Martín Velázquez </t>
-  </si>
-  <si>
-    <t>jorgemartinvelmx@gmail.com</t>
-  </si>
-  <si>
-    <t>Envié correo preguntando que es lo que necesita</t>
-  </si>
-  <si>
-    <t>2020-06-11 01:31:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Guadalupe </t>
-  </si>
-  <si>
-    <t>Andy20ordaz@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-11 00:13:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorena. Gonzalez </t>
-  </si>
-  <si>
-    <t>miriambienesraices@hotmaik.com</t>
-  </si>
-  <si>
-    <t>Envie correo y pregunté si es corredora para ofrecerle la promoción del 4%</t>
-  </si>
-  <si>
-    <t>2020-06-10 20:16:21</t>
-  </si>
-  <si>
-    <t>enicoletarazo@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-10 09:56:57</t>
-  </si>
-  <si>
-    <t>Luis Antonio Duarte</t>
-  </si>
-  <si>
-    <t>luis_duarte34@yahoo.com</t>
-  </si>
-  <si>
-    <t>2020-06-10 09:34:58</t>
-  </si>
-  <si>
-    <t>Diego Salazar</t>
-  </si>
-  <si>
-    <t>diego.sala@live.com.mx</t>
-  </si>
-  <si>
-    <t>Se envió correo desde Kiper.  --  Tiene presupuesto de 4 millones
-le voy a mandar informacion de Nápoles para ver si le interesa</t>
-  </si>
-  <si>
-    <t>2020-06-09 16:38:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitzy </t>
-  </si>
-  <si>
-    <t>nitzysonora@hotmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-09 13:10:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anahid </t>
-  </si>
-  <si>
-    <t>anahidrt@outlook.com</t>
-  </si>
-  <si>
-    <t>2020-06-09 02:42:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dylan Leonardo Bocanegra Aguilar </t>
-  </si>
-  <si>
-    <t>dyl_leon@hotmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-09 00:11:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alfonso Núñez Cruz </t>
-  </si>
-  <si>
-    <t>parmalat27@hotmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-08 23:46:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sergio LC </t>
-  </si>
-  <si>
-    <t>tec_slc@hotmail.com</t>
+    <t>2020-06-20 01:54:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giovanna Abigail </t>
+  </si>
+  <si>
+    <t>giovanna_1175@hotmail.com</t>
+  </si>
+  <si>
+    <t>Envié correo para conocer que necistan.</t>
+  </si>
+  <si>
+    <t>2020-06-19 14:41:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ankita Gandhi </t>
+  </si>
+  <si>
+    <t>ankita.g1983@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envió correo desde Kiper. </t>
+  </si>
+  <si>
+    <t>2020-06-19 13:36:43</t>
+  </si>
+  <si>
+    <t>Francisco Pinilla</t>
+  </si>
+  <si>
+    <t>francisco_pinilla@hotmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-19 11:09:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pamela García </t>
+  </si>
+  <si>
+    <t>pamela.garcia@hotmail.com</t>
   </si>
   <si>
     <t>Envié correo para conocer que necesita</t>
   </si>
   <si>
-    <t>2020-06-08 22:33:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valentina Rodríguez Rodríguez </t>
-  </si>
-  <si>
-    <t>valen.hs@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-08 19:48:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donaldo Herrera </t>
-  </si>
-  <si>
-    <t>d.herreram13@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-08 15:30:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suing Privado Hernández </t>
-  </si>
-  <si>
-    <t>garciahernandezde60@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-08 11:24:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victoria Orvananos </t>
-  </si>
-  <si>
-    <t>victoriaorva@gmail.com</t>
-  </si>
-  <si>
-    <t>2020-06-08 01:50:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel Nava </t>
-  </si>
-  <si>
-    <t>dani.carrasconava@gmail.com</t>
+    <t>2020-06-19 08:13:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura Arratia Ramirez </t>
+  </si>
+  <si>
+    <t>laar_1389@hotmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-18 17:56:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Palomino Renteria </t>
+  </si>
+  <si>
+    <t>interobrabienesyservicios@gmail.com</t>
+  </si>
+  <si>
+    <t>Envié correo para conocer que busca.</t>
+  </si>
+  <si>
+    <t>2020-06-18 11:07:17</t>
+  </si>
+  <si>
+    <t>Roberto De los Santos</t>
+  </si>
+  <si>
+    <t>santos.o.roberto@gamil.com</t>
+  </si>
+  <si>
+    <t>VISITA, quiere arriba de 150 m2 solo que NO quiere VER ningún vecino por su ventana.</t>
+  </si>
+  <si>
+    <t>2020-06-18 08:27:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liliana Piedad </t>
+  </si>
+  <si>
+    <t>licliliana@prodigy.ner.mx</t>
+  </si>
+  <si>
+    <t>2020-06-17 17:57:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana </t>
+  </si>
+  <si>
+    <t>adrinp91@gmail.com</t>
+  </si>
+  <si>
+    <t>Envié correo para saber que busca.</t>
+  </si>
+  <si>
+    <t>2020-06-17 00:53:00</t>
+  </si>
+  <si>
+    <t>etsong0413@hotmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-16 23:16:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduardo Hernández </t>
+  </si>
+  <si>
+    <t>eduardoortigoza535@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-16 21:10:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nayely Fernandez </t>
+  </si>
+  <si>
+    <t>nayely_162@hotmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-16 15:01:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar Ortega </t>
+  </si>
+  <si>
+    <t>argenisortegamx@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-16 12:16:30</t>
+  </si>
+  <si>
+    <t>Jorge Alegre</t>
+  </si>
+  <si>
+    <t>jalegrecapdevielle@icloud.com</t>
+  </si>
+  <si>
+    <t>Esta buscando algo en renta, el día 16 de junio quedo de llegar a las 3 y no llego.
+me dijo que verá su agenda la semana q viene para agendar una cita</t>
+  </si>
+  <si>
+    <t>2020-06-16 11:13:13</t>
+  </si>
+  <si>
+    <t>2020-06-16 05:29:57</t>
+  </si>
+  <si>
+    <t>jaque_vazquez11@hotmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-15 20:59:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karen Martínez Reyes </t>
+  </si>
+  <si>
+    <t>karenmatinesmartinesreyes62@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-06-15 13:13:26</t>
+  </si>
+  <si>
+    <t>benjalinarez@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envié correo para conocer que necesitan. --  RENTA de una sola habitación y presupuesto bajo. </t>
+  </si>
+  <si>
+    <t>2020-06-15 10:25:55</t>
+  </si>
+  <si>
+    <t>Silvia Casco</t>
+  </si>
+  <si>
+    <t>silvia_casco@hotmail.com</t>
+  </si>
+  <si>
+    <t>BROKER externa, envié correo para ofrecer promoción 4% y ver que necesita su cliente.</t>
+  </si>
+  <si>
+    <t>2020-06-15 01:13:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofia Liñero </t>
+  </si>
+  <si>
+    <t>sofia.linero@gmail.com</t>
   </si>
   <si>
     <t>Código de clasificación</t>
@@ -455,65 +355,38 @@
     <t xml:space="preserve">Report Powered by KIPER </t>
   </si>
   <si>
-    <t>Broker</t>
+    <t>Ferlu Davila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaqueline </t>
+  </si>
+  <si>
+    <t>Página Web del Desarrollo</t>
+  </si>
+  <si>
+    <t>Quiere rentar un departamento  --  Se envió correo desde Kiper.</t>
   </si>
   <si>
     <t>Referido</t>
   </si>
   <si>
-    <t xml:space="preserve">Se envió correo desde Kiper.  </t>
-  </si>
-  <si>
-    <t>Se envio correo desde Kiper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isa Ov </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envie correo para conocer que necesita  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para saber que necesita  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para conocer que busca  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para preguntar que es lo que necesita  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para conocer que necesita </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para conocer lo que necesita </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envié correo para conocer que necesita  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se envió correo desde Kiper. </t>
-  </si>
-  <si>
-    <t>Tiene 5 millones de pesos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No contesta envie mail con informacion general  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santiago Perez Amaro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enia Nicole Tarazon Delgado </t>
-  </si>
-  <si>
-    <t>Envié correo para conocer lo que busca</t>
+    <t>Vallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolina Linarez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marisa </t>
+  </si>
+  <si>
+    <t>ferludalo@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -559,6 +432,49 @@
       <color indexed="12"/>
       <name val="Avenir Book"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -580,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -729,9 +645,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -744,6 +681,27 @@
         <color indexed="8"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -751,14 +709,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
+      <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -779,9 +733,16 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -790,9 +751,7 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -820,6 +779,17 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -854,10 +824,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -934,44 +905,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -996,13 +949,14 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1013,22 +967,104 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1166,15 +1202,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>12757</xdr:rowOff>
+      <xdr:colOff>1549400</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>57</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1191,13 +1227,14 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1054100" y="15998825"/>
+          <a:off x="1346200" y="16386175"/>
           <a:ext cx="482600" cy="800158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2293,24 +2330,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV239"/>
+  <dimension ref="A1:IU239"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="14.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="27" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="35.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="168.83203125" style="1" customWidth="1"/>
-    <col min="10" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="255" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2534,7 +2570,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="24">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="23" t="s">
@@ -2553,7 +2589,9 @@
       <c r="E21" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="26"/>
+      <c r="F21" s="26">
+        <v>1</v>
+      </c>
       <c r="G21" s="27"/>
       <c r="H21" s="28"/>
       <c r="I21" s="29"/>
@@ -2567,7 +2605,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="26">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G22" s="27"/>
       <c r="H22" s="28"/>
@@ -2582,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="14"/>
@@ -2601,1172 +2639,964 @@
     </row>
     <row r="25" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="24">
-        <v>17</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="23" t="s">
+      <c r="C25" s="81">
+        <v>12</v>
+      </c>
+      <c r="D25" s="82"/>
+      <c r="E25" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="24">
-        <v>12</v>
-      </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
+      <c r="F25" s="81">
+        <v>3</v>
+      </c>
+      <c r="G25" s="83"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="85"/>
     </row>
     <row r="26" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="24">
-        <v>18</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="24">
-        <v>1</v>
-      </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="15"/>
+      <c r="C26" s="81">
+        <v>11</v>
+      </c>
+      <c r="D26" s="82"/>
+      <c r="E26" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="81">
+        <v>15</v>
+      </c>
+      <c r="G26" s="86"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="88"/>
     </row>
     <row r="27" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="24">
-        <v>21</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="96" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="90">
+        <v>1</v>
+      </c>
+      <c r="G27" s="91"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="88"/>
     </row>
     <row r="28" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F28" s="24">
+      <c r="B28" s="93"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="90">
         <v>1</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="15"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="88"/>
     </row>
     <row r="29" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="90">
+        <v>3</v>
+      </c>
+      <c r="G29" s="100"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="88"/>
     </row>
     <row r="30" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="15"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="88"/>
     </row>
     <row r="31" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="88"/>
     </row>
     <row r="32" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="15"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="107"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="88"/>
     </row>
     <row r="33" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="48" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="F33" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="G33" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="48" t="s">
+      <c r="H33" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="50" t="s">
+      <c r="I33" s="111" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="40">
+      <c r="A34" s="41">
         <v>1</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="101" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="113">
+        <v>5525587376</v>
+      </c>
+      <c r="H34" s="101" t="s">
+        <v>58</v>
+      </c>
+      <c r="I34" s="114" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="41">
+        <v>2</v>
+      </c>
+      <c r="B35" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="113">
+        <v>9991851229</v>
+      </c>
+      <c r="H35" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="41">
+        <v>3</v>
+      </c>
+      <c r="B36" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="113">
+        <v>8331047641</v>
+      </c>
+      <c r="H36" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <v>4</v>
+      </c>
+      <c r="B37" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="101" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="101" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="113">
+        <v>3331199618</v>
+      </c>
+      <c r="H37" s="101" t="s">
+        <v>77</v>
+      </c>
+      <c r="I37" s="114" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="41">
+        <v>5</v>
+      </c>
+      <c r="B38" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="101" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="113">
+        <v>5520736850</v>
+      </c>
+      <c r="H38" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" s="114" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="41">
+        <v>6</v>
+      </c>
+      <c r="B39" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="101" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="113">
+        <v>7226006011</v>
+      </c>
+      <c r="H39" s="101" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="41">
+        <v>7</v>
+      </c>
+      <c r="B40" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" s="51" t="s">
+      <c r="G40" s="113">
+        <v>7713198299</v>
+      </c>
+      <c r="H40" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="40">
-        <v>5548801304</v>
-      </c>
-      <c r="H34" s="51" t="s">
+      <c r="I40" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="I34" s="51" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53">
-        <v>2</v>
-      </c>
-      <c r="B35" s="51" t="s">
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="41">
+        <v>8</v>
+      </c>
+      <c r="B41" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C41" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="51" t="s">
+      <c r="D41" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="101" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="113">
+        <v>5520928132</v>
+      </c>
+      <c r="H41" s="101" t="s">
+        <v>47</v>
+      </c>
+      <c r="I41" s="114" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="41">
         <v>9</v>
       </c>
-      <c r="F35" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="40">
-        <v>5573378033</v>
-      </c>
-      <c r="H35" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="I35" s="51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54">
-        <v>3</v>
-      </c>
-      <c r="B36" s="51" t="s">
+      <c r="B42" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="113">
+        <v>2225296479</v>
+      </c>
+      <c r="H42" s="101" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="41">
+        <v>10</v>
+      </c>
+      <c r="B43" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C43" s="101" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" s="113">
+        <v>3141497974</v>
+      </c>
+      <c r="H43" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="114" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="41">
+        <v>11</v>
+      </c>
+      <c r="B44" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="51" t="s">
+      <c r="D44" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="40">
-        <v>8180292291</v>
-      </c>
-      <c r="H36" s="51" t="s">
+      <c r="G44" s="113">
+        <v>5522993373</v>
+      </c>
+      <c r="H44" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="I36" s="51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
-        <v>4</v>
-      </c>
-      <c r="B37" s="51" t="s">
+      <c r="I44" s="114" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="41">
+        <v>12</v>
+      </c>
+      <c r="B45" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="101" t="s">
+        <v>115</v>
+      </c>
+      <c r="G45" s="113">
+        <v>55133378245</v>
+      </c>
+      <c r="H45" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="114" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="41">
+        <v>13</v>
+      </c>
+      <c r="B46" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C46" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="51" t="s">
+      <c r="G46" s="113">
+        <v>5612586813</v>
+      </c>
+      <c r="H46" s="101" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="40">
-        <v>5540217314</v>
-      </c>
-      <c r="H37" s="51" t="s">
+      <c r="I46" s="114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="41">
+        <v>14</v>
+      </c>
+      <c r="B47" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="I37" s="51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53">
-        <v>5</v>
-      </c>
-      <c r="B38" s="51" t="s">
+      <c r="D47" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="101" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="113">
+        <v>4434406385</v>
+      </c>
+      <c r="H47" s="101" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="41">
+        <v>15</v>
+      </c>
+      <c r="B48" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="101" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="101" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="113">
+        <v>8123242144</v>
+      </c>
+      <c r="H48" s="115" t="s">
+        <v>116</v>
+      </c>
+      <c r="I48" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="41">
+        <v>16</v>
+      </c>
+      <c r="B49" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C49" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="51" t="s">
+      <c r="D49" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="101" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" s="113">
+        <v>2292066866</v>
+      </c>
+      <c r="H49" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="G38" s="40">
-        <v>9994867755</v>
-      </c>
-      <c r="H38" s="51" t="s">
+      <c r="I49" s="114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="41">
+        <v>17</v>
+      </c>
+      <c r="B50" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="I38" s="51" t="s">
+      <c r="D50" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="101" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54">
-        <v>6</v>
-      </c>
-      <c r="B39" s="51" t="s">
+      <c r="G50" s="113">
+        <v>5617118889</v>
+      </c>
+      <c r="H50" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="I50" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="41">
+        <v>18</v>
+      </c>
+      <c r="B51" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="113">
+        <v>5585800790</v>
+      </c>
+      <c r="H51" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="I51" s="114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="41">
+        <v>19</v>
+      </c>
+      <c r="B52" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="51" t="s">
+      <c r="C52" s="101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="113">
+        <v>5533582474</v>
+      </c>
+      <c r="H52" s="101" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" s="114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="41">
+        <v>20</v>
+      </c>
+      <c r="B53" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="113">
+        <v>7772748682</v>
+      </c>
+      <c r="H53" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="I53" s="114" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="41">
+        <v>21</v>
+      </c>
+      <c r="B54" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="101" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="113">
+        <v>9842797524</v>
+      </c>
+      <c r="H54" s="101" t="s">
+        <v>89</v>
+      </c>
+      <c r="I54" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" s="40">
-        <v>7228848742</v>
-      </c>
-      <c r="H39" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40">
-        <v>7</v>
-      </c>
-      <c r="B40" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E40" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="G40" s="40">
-        <v>6121544983</v>
-      </c>
-      <c r="H40" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" s="51" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53">
-        <v>8</v>
-      </c>
-      <c r="B41" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="40">
-        <v>4441112233</v>
-      </c>
-      <c r="H41" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54">
-        <v>9</v>
-      </c>
-      <c r="B42" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="G42" s="40">
-        <v>3921110352</v>
-      </c>
-      <c r="H42" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="I42" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="40">
-        <v>10</v>
-      </c>
-      <c r="B43" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="51" t="s">
+    </row>
+    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="41">
+        <v>22</v>
+      </c>
+      <c r="B55" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="101" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="101" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="113">
+        <v>5514868979</v>
+      </c>
+      <c r="H55" s="101" t="s">
+        <v>80</v>
+      </c>
+      <c r="I55" s="116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="42">
+        <v>23</v>
+      </c>
+      <c r="B56" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E43" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="G43" s="40">
-        <v>7444215567</v>
-      </c>
-      <c r="H43" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="I43" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="53">
-        <v>11</v>
-      </c>
-      <c r="B44" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E44" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="G44" s="40">
-        <v>7713960739</v>
-      </c>
-      <c r="H44" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="I44" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54">
-        <v>12</v>
-      </c>
-      <c r="B45" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="G45" s="40">
-        <v>3325923224</v>
-      </c>
-      <c r="H45" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="I45" s="51" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="40">
-        <v>13</v>
-      </c>
-      <c r="B46" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="40">
-        <v>5528585800</v>
-      </c>
-      <c r="H46" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" s="51" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53">
-        <v>14</v>
-      </c>
-      <c r="B47" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="G47" s="40">
-        <v>2226647393</v>
-      </c>
-      <c r="H47" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="I47" s="51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54">
-        <v>15</v>
-      </c>
-      <c r="B48" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E48" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="G48" s="40">
-        <v>5611131335</v>
-      </c>
-      <c r="H48" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="I48" s="51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="40">
-        <v>16</v>
-      </c>
-      <c r="B49" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="G49" s="40">
-        <v>5524142623</v>
-      </c>
-      <c r="H49" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="I49" s="51" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="53">
-        <v>17</v>
-      </c>
-      <c r="B50" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E50" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="G50" s="40">
-        <v>7221009888</v>
-      </c>
-      <c r="H50" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="I50" s="51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54">
-        <v>18</v>
-      </c>
-      <c r="B51" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E51" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="G51" s="40">
-        <v>8332859407</v>
-      </c>
-      <c r="H51" s="51" t="s">
+      <c r="F56" s="101" t="s">
+        <v>43</v>
+      </c>
+      <c r="G56" s="113">
+        <v>5549505622</v>
+      </c>
+      <c r="H56" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="I56" s="114" t="s">
         <v>111</v>
       </c>
-      <c r="I51" s="51" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="40">
-        <v>19</v>
-      </c>
-      <c r="B52" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E52" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="G52" s="40">
-        <v>5554070688</v>
-      </c>
-      <c r="H52" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="I52" s="51" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="53">
-        <v>20</v>
-      </c>
-      <c r="B53" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="D53" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" s="40">
-        <v>5588050507</v>
-      </c>
-      <c r="H53" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="I53" s="51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54">
-        <v>21</v>
-      </c>
-      <c r="B54" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="G54" s="40">
-        <v>8311597993</v>
-      </c>
-      <c r="H54" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="I54" s="44" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="40">
-        <v>22</v>
-      </c>
-      <c r="B55" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="G55" s="40">
-        <v>1560360634</v>
-      </c>
-      <c r="H55" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="I55" s="51" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="53">
-        <v>23</v>
-      </c>
-      <c r="B56" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="G56" s="40">
-        <v>9988201805</v>
-      </c>
-      <c r="H56" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="I56" s="51" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="57" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="54">
-        <v>24</v>
-      </c>
-      <c r="B57" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E57" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="G57" s="40">
-        <v>9981578793</v>
-      </c>
-      <c r="H57" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="I57" s="51" t="s">
-        <v>156</v>
-      </c>
+      <c r="A57" s="40"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
     </row>
     <row r="58" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="40">
-        <v>25</v>
-      </c>
-      <c r="B58" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E58" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="G58" s="40">
-        <v>3022416623</v>
-      </c>
-      <c r="H58" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="I58" s="51" t="s">
-        <v>146</v>
-      </c>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53">
-        <v>26</v>
-      </c>
-      <c r="B59" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="D59" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E59" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="G59" s="40">
-        <v>4421794890</v>
-      </c>
-      <c r="H59" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="I59" s="51" t="s">
-        <v>146</v>
-      </c>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
     </row>
     <row r="60" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54">
-        <v>27</v>
-      </c>
-      <c r="B60" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E60" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="51" t="s">
-        <v>160</v>
-      </c>
-      <c r="G60" s="40">
-        <v>6121373285</v>
-      </c>
-      <c r="H60" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="I60" s="51" t="s">
-        <v>146</v>
-      </c>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="40"/>
     </row>
     <row r="61" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40">
-        <v>28</v>
-      </c>
-      <c r="B61" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="D61" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E61" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="G61" s="40">
-        <v>5610531758</v>
-      </c>
-      <c r="H61" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="I61" s="51" t="s">
-        <v>146</v>
-      </c>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="40"/>
     </row>
     <row r="62" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="53">
-        <v>29</v>
-      </c>
-      <c r="B62" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="G62" s="40">
-        <v>5678901235</v>
-      </c>
-      <c r="H62" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="I62" s="51" t="s">
-        <v>146</v>
-      </c>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
     </row>
     <row r="63" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="54">
-        <v>30</v>
-      </c>
-      <c r="B63" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D63" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G63" s="40">
-        <v>5616164729</v>
-      </c>
-      <c r="H63" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="I63" s="51" t="s">
-        <v>44</v>
-      </c>
+      <c r="A63" s="40"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
     </row>
     <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40">
-        <v>31</v>
-      </c>
-      <c r="B64" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E64" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="F64" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="G64" s="40">
-        <v>5551279866</v>
-      </c>
-      <c r="H64" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="I64" s="51" t="s">
-        <v>69</v>
-      </c>
+      <c r="A64" s="40"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="53">
-        <v>32</v>
-      </c>
-      <c r="B65" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="E65" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="G65" s="40">
-        <v>5563536081</v>
-      </c>
-      <c r="H65" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="I65" s="55" t="s">
-        <v>102</v>
-      </c>
+      <c r="A65" s="40"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
     </row>
     <row r="66" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54">
-        <v>33</v>
-      </c>
-      <c r="B66" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="E66" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="G66" s="44"/>
-      <c r="H66" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="I66" s="51" t="s">
-        <v>79</v>
-      </c>
+      <c r="A66" s="40"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
+      <c r="I66" s="40"/>
     </row>
     <row r="67" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="40">
-        <v>34</v>
-      </c>
-      <c r="B67" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="51" t="s">
-        <v>159</v>
-      </c>
-      <c r="G67" s="44"/>
-      <c r="H67" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="I67" s="44" t="s">
-        <v>147</v>
-      </c>
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="40"/>
     </row>
     <row r="68" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="53">
-        <v>35</v>
-      </c>
-      <c r="B68" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="D68" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="G68" s="40">
-        <v>9212625458</v>
-      </c>
-      <c r="H68" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="51" t="s">
-        <v>157</v>
-      </c>
+      <c r="A68" s="46"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="49"/>
     </row>
     <row r="69" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="57"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="7"/>
     </row>
     <row r="70" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
-      <c r="D70" s="58"/>
+      <c r="D70" s="50"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -3777,7 +3607,7 @@
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="58"/>
+      <c r="D71" s="50"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
@@ -3786,119 +3616,119 @@
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="B72" s="59"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="60"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="52"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
-      <c r="B73" s="61" t="s">
-        <v>134</v>
-      </c>
-      <c r="C73" s="62"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
+      <c r="B73" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C73" s="54"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
       <c r="G73" s="17"/>
-      <c r="H73" s="64"/>
-      <c r="I73" s="65"/>
+      <c r="H73" s="56"/>
+      <c r="I73" s="57"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="62"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="63"/>
-      <c r="F74" s="63"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="55"/>
       <c r="G74" s="17"/>
-      <c r="H74" s="64"/>
-      <c r="I74" s="65"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="57"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
-      <c r="B75" s="66"/>
-      <c r="C75" s="67"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="66"/>
-      <c r="F75" s="66"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="65"/>
+      <c r="B75" s="58"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="58"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58"/>
+      <c r="G75" s="60"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="57"/>
     </row>
     <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
-      <c r="B76" s="69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C76" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" s="71"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="73"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="76"/>
+      <c r="B76" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D76" s="64"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="67"/>
+      <c r="H76" s="68"/>
+      <c r="I76" s="69"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
-      <c r="B77" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="C77" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="D77" s="71"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="74"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="76"/>
+      <c r="B77" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D77" s="64"/>
+      <c r="E77" s="65"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
+      <c r="H77" s="68"/>
+      <c r="I77" s="69"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
-      <c r="B78" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="C78" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="D78" s="71"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="73"/>
-      <c r="G78" s="74"/>
-      <c r="H78" s="75"/>
-      <c r="I78" s="76"/>
+      <c r="B78" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" s="64"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="67"/>
+      <c r="H78" s="68"/>
+      <c r="I78" s="69"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
-      <c r="B79" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="C79" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="D79" s="71"/>
-      <c r="E79" s="72"/>
-      <c r="F79" s="72"/>
-      <c r="G79" s="77"/>
-      <c r="H79" s="78"/>
-      <c r="I79" s="79"/>
+      <c r="B79" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="C79" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" s="64"/>
+      <c r="E79" s="65"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="70"/>
+      <c r="H79" s="71"/>
+      <c r="I79" s="72"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="45"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="45"/>
-      <c r="H80" s="45"/>
+      <c r="B80" s="73"/>
+      <c r="C80" s="73"/>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="73"/>
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3947,8 +3777,8 @@
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="80" t="s">
-        <v>143</v>
+      <c r="B85" s="75" t="s">
+        <v>107</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
@@ -5642,25 +5472,28 @@
       <c r="I238" s="7"/>
     </row>
     <row r="239" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="81"/>
-      <c r="B239" s="82"/>
-      <c r="C239" s="82"/>
-      <c r="D239" s="82"/>
-      <c r="E239" s="82"/>
-      <c r="F239" s="83"/>
-      <c r="G239" s="82"/>
-      <c r="H239" s="82"/>
-      <c r="I239" s="84"/>
+      <c r="A239" s="76"/>
+      <c r="B239" s="77"/>
+      <c r="C239" s="77"/>
+      <c r="D239" s="77"/>
+      <c r="E239" s="77"/>
+      <c r="F239" s="78"/>
+      <c r="G239" s="77"/>
+      <c r="H239" s="77"/>
+      <c r="I239" s="79"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:A68">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:A56">
     <sortCondition ref="A34"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="H48" r:id="rId1" xr:uid="{3873D696-06F3-4C6A-8BE1-D177FEC5C112}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup scale="80" orientation="landscape"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>